<commit_message>
Added recursive and iterative sorts comparison
</commit_message>
<xml_diff>
--- a/results/radix.xlsx
+++ b/results/radix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s\PycharmProjects\sorts\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{90B75E96-7DD4-4E11-86DF-45D80FBFC323}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B46685B7-3E74-4DA6-8C9A-F36215D7ED9C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="straight" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -487,7 +489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -566,7 +570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -645,7 +651,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -722,13 +730,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48863D98-D2F2-421D-8DD6-F68F79212A2C}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>5</v>
       </c>
@@ -744,45 +754,54 @@
       <c r="F1">
         <v>50000</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.0029999999999996E-3</v>
+        <v>3.503E-3</v>
       </c>
       <c r="C2">
-        <v>3.3033E-2</v>
+        <v>1.8519999999999998E-2</v>
       </c>
       <c r="D2">
-        <v>0.384903</v>
+        <v>0.19019900000000001</v>
       </c>
       <c r="E2">
-        <v>2.3812120000000001</v>
+        <v>1.8714550000000001</v>
       </c>
       <c r="F2">
-        <v>24.266970000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21.047982999999999</v>
+      </c>
+      <c r="G2">
+        <v>206.405991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6.0060000000000001E-3</v>
+        <v>4.5050000000000003E-3</v>
       </c>
       <c r="C3">
-        <v>3.4535999999999997E-2</v>
+        <v>1.7517000000000001E-2</v>
       </c>
       <c r="D3">
-        <v>0.28824</v>
+        <v>0.22573599999999999</v>
       </c>
       <c r="E3">
-        <v>2.4252150000000001</v>
+        <v>1.8399220000000001</v>
       </c>
       <c r="F3">
-        <v>26.466301000000001</v>
+        <v>22.778307999999999</v>
+      </c>
+      <c r="G3">
+        <v>229.372907</v>
       </c>
     </row>
   </sheetData>
@@ -792,15 +811,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745B6391-B7DC-4BA9-8F74-271F36AED3B8}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>5</v>
       </c>
@@ -816,45 +835,54 @@
       <c r="F1">
         <v>50000</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.0000000000000001E-3</v>
+        <v>3.003E-3</v>
       </c>
       <c r="C2">
-        <v>1.6036000000000002E-2</v>
+        <v>1.8519000000000001E-2</v>
       </c>
       <c r="D2">
-        <v>0.14002700000000001</v>
+        <v>0.229739</v>
       </c>
       <c r="E2">
-        <v>1.4141600000000001</v>
+        <v>2.4205290000000002</v>
       </c>
       <c r="F2">
-        <v>14.362453</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21.456924999999998</v>
+      </c>
+      <c r="G2">
+        <v>221.834946</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3.0010000000000002E-3</v>
+        <v>4.5050000000000003E-3</v>
       </c>
       <c r="C3">
-        <v>1.3988E-2</v>
+        <v>2.2023000000000001E-2</v>
       </c>
       <c r="D3">
-        <v>0.147977</v>
+        <v>0.24926000000000001</v>
       </c>
       <c r="E3">
-        <v>1.426091</v>
+        <v>2.188285</v>
       </c>
       <c r="F3">
-        <v>16.179431000000001</v>
+        <v>22.878900000000002</v>
+      </c>
+      <c r="G3">
+        <v>229.67623900000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>